<commit_message>
Remove deprecation, and instead only remove nanoDESI
</commit_message>
<xml_diff>
--- a/docs/nano/nano-metadata.xlsx
+++ b/docs/nano/nano-metadata.xlsx
@@ -396,7 +396,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>version</t>
   </si>
@@ -438,9 +438,6 @@
   </si>
   <si>
     <t>assay_type</t>
-  </si>
-  <si>
-    <t>NanoDESI</t>
   </si>
   <si>
     <t>NanoPOTS</t>
@@ -917,52 +914,52 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -973,8 +970,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mass_spectrometry_imaging." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: NanoDESI / NanoPOTS." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: NanoPOTS." sqref="L2:L1048576">
+      <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: metabolites_and_lipids." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1054,7 +1051,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1063,11 +1060,6 @@
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1077,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1103,27 +1095,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1141,12 +1133,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1164,12 +1156,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1187,12 +1179,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Remove deprecation, and instead only remove nanoDESI"
This reverts commit 7372e1bee00fc5cb9339803b4dca05eabc911bb5.
</commit_message>
<xml_diff>
--- a/docs/nano/nano-metadata.xlsx
+++ b/docs/nano/nano-metadata.xlsx
@@ -396,7 +396,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>version</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>assay_type</t>
+  </si>
+  <si>
+    <t>NanoDESI</t>
   </si>
   <si>
     <t>NanoPOTS</t>
@@ -914,52 +917,52 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -970,8 +973,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mass_spectrometry_imaging." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: NanoPOTS." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$1</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: NanoDESI / NanoPOTS." sqref="L2:L1048576">
+      <formula1>'assay_type list'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: metabolites_and_lipids." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1051,7 +1054,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1060,6 +1063,11 @@
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1077,7 +1085,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1095,27 +1103,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1133,12 +1141,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1156,12 +1164,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1179,12 +1187,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>